<commit_message>
fix(allowance): issue on import allowance generate payroll
</commit_message>
<xml_diff>
--- a/build/assets/templates/allowance.xlsx
+++ b/build/assets/templates/allowance.xlsx
@@ -32,7 +32,7 @@
     <t>Nominal</t>
   </si>
   <si>
-    <t>Employee id</t>
+    <t>Employee Id</t>
   </si>
 </sst>
 </file>
@@ -68,8 +68,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -353,12 +354,12 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -366,7 +367,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
@@ -378,5 +379,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(indonesian): change language to indonesian
</commit_message>
<xml_diff>
--- a/build/assets/templates/allowance.xlsx
+++ b/build/assets/templates/allowance.xlsx
@@ -32,7 +32,7 @@
     <t>Nominal</t>
   </si>
   <si>
-    <t>Employee Id</t>
+    <t>NIP</t>
   </si>
 </sst>
 </file>
@@ -354,7 +354,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>